<commit_message>
KeyError son kez duzeltildi
</commit_message>
<xml_diff>
--- a/analitik_veri.xlsx
+++ b/analitik_veri.xlsx
@@ -24,9 +24,6 @@
     <t>Molekül Adı</t>
   </si>
   <si>
-    <t>İlaç Grubu</t>
-  </si>
-  <si>
     <t>Analiz Matriksi</t>
   </si>
   <si>
@@ -964,6 +961,9 @@
   </si>
   <si>
     <t>Orijinal ürün ile biyobenzerin kritik kalite özelliklerinin (CQA) ve primer/sekonder yapılarının karşılaştırılması.</t>
+  </si>
+  <si>
+    <t>Molekül Tipi</t>
   </si>
 </sst>
 </file>
@@ -1256,332 +1256,332 @@
   </sheetPr>
   <dimension ref="A1:Z62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="A63" sqref="A63"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="1" t="s">
+    </row>
+    <row r="3" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="E3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="E4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="1" t="s">
+      <c r="E9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F10" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="E12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>69</v>
-      </c>
       <c r="G12" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="E13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13" s="1" t="s">
+      <c r="G13" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="C14" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="E14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E14" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F14" s="2" t="s">
+      <c r="G14" s="3" t="s">
         <v>80</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>81</v>
       </c>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
@@ -1605,25 +1605,25 @@
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D15" s="2" t="s">
+      <c r="E15" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F15" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="E15" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>84</v>
-      </c>
       <c r="G15" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
@@ -1647,25 +1647,25 @@
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="C16" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D16" s="2" t="s">
+      <c r="E16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="E16" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F16" s="2" t="s">
+      <c r="G16" s="3" t="s">
         <v>88</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>89</v>
       </c>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
@@ -1689,25 +1689,25 @@
     </row>
     <row r="17" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="C17" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="D17" s="2" t="s">
+      <c r="E17" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F17" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="E17" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F17" s="2" t="s">
+      <c r="G17" s="3" t="s">
         <v>93</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>94</v>
       </c>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
@@ -1731,25 +1731,25 @@
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="C18" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="D18" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F18" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="F18" s="2" t="s">
+      <c r="G18" s="3" t="s">
         <v>98</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>99</v>
       </c>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
@@ -1773,25 +1773,25 @@
     </row>
     <row r="19" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="C19" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="D19" s="2" t="s">
+      <c r="E19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="E19" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F19" s="2" t="s">
+      <c r="G19" s="3" t="s">
         <v>103</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>104</v>
       </c>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
@@ -1815,25 +1815,25 @@
     </row>
     <row r="20" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="C20" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F20" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>107</v>
-      </c>
       <c r="G20" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
@@ -1857,25 +1857,25 @@
     </row>
     <row r="21" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="C21" s="2" t="s">
+      <c r="D21" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="E21" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F21" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="E21" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F21" s="2" t="s">
+      <c r="G21" s="3" t="s">
         <v>111</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>112</v>
       </c>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
@@ -1899,25 +1899,25 @@
     </row>
     <row r="22" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="C22" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D22" s="2" t="s">
+      <c r="E22" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="F22" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="G22" s="3" t="s">
         <v>117</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>118</v>
       </c>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
@@ -1941,25 +1941,25 @@
     </row>
     <row r="23" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C23" s="2" t="s">
+      <c r="D23" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="E23" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="E23" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F23" s="2" t="s">
+      <c r="G23" s="3" t="s">
         <v>122</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>123</v>
       </c>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
@@ -1983,25 +1983,25 @@
     </row>
     <row r="24" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D24" s="2" t="s">
+      <c r="E24" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F24" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="E24" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="F24" s="2" t="s">
+      <c r="G24" s="2" t="s">
         <v>126</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>127</v>
       </c>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
@@ -2025,25 +2025,25 @@
     </row>
     <row r="25" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C25" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D25" s="2" t="s">
-        <v>79</v>
-      </c>
       <c r="E25" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
@@ -2067,25 +2067,25 @@
     </row>
     <row r="26" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="D26" s="2" t="s">
+      <c r="E26" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F26" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="E26" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>131</v>
-      </c>
       <c r="G26" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
@@ -2109,25 +2109,25 @@
     </row>
     <row r="27" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F27" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>133</v>
-      </c>
       <c r="G27" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
@@ -2151,25 +2151,25 @@
     </row>
     <row r="28" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F28" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F28" s="2" t="s">
+      <c r="G28" s="3" t="s">
         <v>135</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>136</v>
       </c>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
@@ -2193,25 +2193,25 @@
     </row>
     <row r="29" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="C29" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="D29" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F29" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="D29" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F29" s="2" t="s">
+      <c r="G29" s="3" t="s">
         <v>140</v>
-      </c>
-      <c r="G29" s="3" t="s">
-        <v>141</v>
       </c>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
@@ -2235,25 +2235,25 @@
     </row>
     <row r="30" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="C30" s="2" t="s">
+      <c r="D30" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="E30" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="E30" s="2" t="s">
+      <c r="F30" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="F30" s="2" t="s">
+      <c r="G30" s="3" t="s">
         <v>146</v>
-      </c>
-      <c r="G30" s="3" t="s">
-        <v>147</v>
       </c>
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
@@ -2277,25 +2277,25 @@
     </row>
     <row r="31" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="C31" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F31" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="C31" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F31" s="2" t="s">
+      <c r="G31" s="3" t="s">
         <v>150</v>
-      </c>
-      <c r="G31" s="3" t="s">
-        <v>151</v>
       </c>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
@@ -2319,25 +2319,25 @@
     </row>
     <row r="32" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="C32" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="D32" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="E32" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="E32" s="2" t="s">
+      <c r="F32" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="F32" s="2" t="s">
+      <c r="G32" s="3" t="s">
         <v>157</v>
-      </c>
-      <c r="G32" s="3" t="s">
-        <v>158</v>
       </c>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
@@ -2361,25 +2361,25 @@
     </row>
     <row r="33" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="C33" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="D33" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F33" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="D33" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="F33" s="2" t="s">
+      <c r="G33" s="2" t="s">
         <v>162</v>
-      </c>
-      <c r="G33" s="2" t="s">
-        <v>163</v>
       </c>
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
@@ -2403,25 +2403,25 @@
     </row>
     <row r="34" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="C34" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="D34" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="E34" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F34" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="E34" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F34" s="2" t="s">
+      <c r="G34" s="3" t="s">
         <v>168</v>
-      </c>
-      <c r="G34" s="3" t="s">
-        <v>169</v>
       </c>
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
@@ -2445,25 +2445,25 @@
     </row>
     <row r="35" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="C35" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="D35" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="F35" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="D35" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>173</v>
-      </c>
       <c r="G35" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
@@ -2487,25 +2487,25 @@
     </row>
     <row r="36" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="C36" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F36" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="C36" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>176</v>
-      </c>
       <c r="G36" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
@@ -2529,25 +2529,25 @@
     </row>
     <row r="37" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="C37" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="D37" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="E37" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="E37" s="2" t="s">
+      <c r="F37" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="F37" s="2" t="s">
+      <c r="G37" s="3" t="s">
         <v>182</v>
-      </c>
-      <c r="G37" s="3" t="s">
-        <v>183</v>
       </c>
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
@@ -2571,25 +2571,25 @@
     </row>
     <row r="38" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="C38" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="D38" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="D38" s="2" t="s">
+      <c r="E38" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F38" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="E38" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>188</v>
-      </c>
       <c r="G38" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H38" s="2"/>
       <c r="I38" s="2"/>
@@ -2613,25 +2613,25 @@
     </row>
     <row r="39" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B39" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="C39" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="D39" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="E39" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F39" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="E39" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>193</v>
-      </c>
       <c r="G39" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H39" s="2"/>
       <c r="I39" s="2"/>
@@ -2655,25 +2655,25 @@
     </row>
     <row r="40" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B40" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="C40" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="D40" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="D40" s="2" t="s">
+      <c r="E40" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="E40" s="2" t="s">
+      <c r="F40" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="F40" s="2" t="s">
+      <c r="G40" s="3" t="s">
         <v>199</v>
-      </c>
-      <c r="G40" s="3" t="s">
-        <v>200</v>
       </c>
       <c r="H40" s="2"/>
       <c r="I40" s="2"/>
@@ -2697,25 +2697,25 @@
     </row>
     <row r="41" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B41" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="C41" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D41" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="C41" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D41" s="2" t="s">
+      <c r="E41" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F41" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="E41" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>204</v>
-      </c>
       <c r="G41" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H41" s="2"/>
       <c r="I41" s="2"/>
@@ -2739,25 +2739,25 @@
     </row>
     <row r="42" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="B42" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="C42" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D42" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="C42" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="D42" s="2" t="s">
+      <c r="E42" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F42" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="E42" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="F42" s="2" t="s">
-        <v>208</v>
-      </c>
       <c r="G42" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H42" s="2"/>
       <c r="I42" s="2"/>
@@ -2781,25 +2781,25 @@
     </row>
     <row r="43" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="B43" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="C43" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="D43" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="E43" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="D43" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="E43" s="2" t="s">
+      <c r="F43" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="F43" s="2" t="s">
-        <v>213</v>
-      </c>
       <c r="G43" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H43" s="2"/>
       <c r="I43" s="2"/>
@@ -2823,25 +2823,25 @@
     </row>
     <row r="44" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="B44" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="C44" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="D44" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="F44" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="D44" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F44" s="2" t="s">
+      <c r="G44" s="3" t="s">
         <v>217</v>
-      </c>
-      <c r="G44" s="3" t="s">
-        <v>218</v>
       </c>
       <c r="H44" s="2"/>
       <c r="I44" s="2"/>
@@ -2865,25 +2865,25 @@
     </row>
     <row r="45" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B45" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="C45" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="D45" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F45" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="D45" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F45" s="2" t="s">
+      <c r="G45" s="3" t="s">
         <v>222</v>
-      </c>
-      <c r="G45" s="3" t="s">
-        <v>223</v>
       </c>
       <c r="H45" s="2"/>
       <c r="I45" s="2"/>
@@ -2907,25 +2907,25 @@
     </row>
     <row r="46" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="B46" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="C46" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D46" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="C46" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D46" s="2" t="s">
+      <c r="E46" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="E46" s="2" t="s">
+      <c r="F46" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="F46" s="2" t="s">
+      <c r="G46" s="3" t="s">
         <v>228</v>
-      </c>
-      <c r="G46" s="3" t="s">
-        <v>229</v>
       </c>
       <c r="H46" s="2"/>
       <c r="I46" s="2"/>
@@ -2949,25 +2949,25 @@
     </row>
     <row r="47" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="B47" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="C47" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="D47" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="D47" s="2" t="s">
+      <c r="E47" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F47" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="E47" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F47" s="2" t="s">
-        <v>234</v>
-      </c>
       <c r="G47" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H47" s="2"/>
       <c r="I47" s="2"/>
@@ -2991,25 +2991,25 @@
     </row>
     <row r="48" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="B48" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="C48" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="C48" s="2" t="s">
+      <c r="D48" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="D48" s="2" t="s">
+      <c r="E48" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="E48" s="2" t="s">
+      <c r="F48" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="F48" s="2" t="s">
-        <v>240</v>
-      </c>
       <c r="G48" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H48" s="2"/>
       <c r="I48" s="2"/>
@@ -3033,25 +3033,25 @@
     </row>
     <row r="49" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="B49" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="C49" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="D49" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="C49" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="D49" s="2" t="s">
+      <c r="E49" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="F49" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="E49" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="F49" s="2" t="s">
-        <v>244</v>
-      </c>
       <c r="G49" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H49" s="2"/>
       <c r="I49" s="2"/>
@@ -3075,25 +3075,25 @@
     </row>
     <row r="50" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="B50" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="C50" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="C50" s="2" t="s">
+      <c r="D50" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="D50" s="2" t="s">
+      <c r="E50" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="E50" s="2" t="s">
+      <c r="F50" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="F50" s="2" t="s">
+      <c r="G50" s="3" t="s">
         <v>250</v>
-      </c>
-      <c r="G50" s="3" t="s">
-        <v>251</v>
       </c>
       <c r="H50" s="2"/>
       <c r="I50" s="2"/>
@@ -3117,25 +3117,25 @@
     </row>
     <row r="51" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="B51" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="C51" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="C51" s="2" t="s">
+      <c r="D51" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="D51" s="2" t="s">
+      <c r="E51" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="F51" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="E51" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F51" s="2" t="s">
-        <v>256</v>
-      </c>
       <c r="G51" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H51" s="2"/>
       <c r="I51" s="2"/>
@@ -3159,25 +3159,25 @@
     </row>
     <row r="52" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="B52" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="C52" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D52" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="C52" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="D52" s="2" t="s">
+      <c r="E52" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="E52" s="2" t="s">
+      <c r="F52" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="F52" s="2" t="s">
+      <c r="G52" s="3" t="s">
         <v>261</v>
-      </c>
-      <c r="G52" s="3" t="s">
-        <v>262</v>
       </c>
       <c r="H52" s="2"/>
       <c r="I52" s="2"/>
@@ -3201,25 +3201,25 @@
     </row>
     <row r="53" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="B53" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="C53" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="C53" s="2" t="s">
+      <c r="D53" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="D53" s="2" t="s">
+      <c r="E53" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F53" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="E53" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="F53" s="2" t="s">
+      <c r="G53" s="3" t="s">
         <v>267</v>
-      </c>
-      <c r="G53" s="3" t="s">
-        <v>268</v>
       </c>
       <c r="H53" s="2"/>
       <c r="I53" s="2"/>
@@ -3243,25 +3243,25 @@
     </row>
     <row r="54" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="B54" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="C54" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D54" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="C54" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D54" s="2" t="s">
+      <c r="E54" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F54" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="E54" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F54" s="2" t="s">
-        <v>272</v>
-      </c>
       <c r="G54" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H54" s="2"/>
       <c r="I54" s="2"/>
@@ -3285,25 +3285,25 @@
     </row>
     <row r="55" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="B55" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="C55" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D55" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="C55" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D55" s="2" t="s">
+      <c r="E55" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="E55" s="2" t="s">
+      <c r="F55" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="F55" s="2" t="s">
+      <c r="G55" s="3" t="s">
         <v>277</v>
-      </c>
-      <c r="G55" s="3" t="s">
-        <v>278</v>
       </c>
       <c r="H55" s="2"/>
       <c r="I55" s="2"/>
@@ -3327,25 +3327,25 @@
     </row>
     <row r="56" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="B56" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="C56" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="C56" s="2" t="s">
+      <c r="D56" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="D56" s="2" t="s">
+      <c r="E56" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F56" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="E56" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="F56" s="2" t="s">
+      <c r="G56" s="2" t="s">
         <v>283</v>
-      </c>
-      <c r="G56" s="2" t="s">
-        <v>284</v>
       </c>
       <c r="H56" s="2"/>
       <c r="I56" s="2"/>
@@ -3369,25 +3369,25 @@
     </row>
     <row r="57" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="B57" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="C57" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="D57" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="C57" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="D57" s="2" t="s">
+      <c r="E57" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="E57" s="2" t="s">
+      <c r="F57" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="F57" s="2" t="s">
-        <v>289</v>
-      </c>
       <c r="G57" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H57" s="2"/>
       <c r="I57" s="2"/>
@@ -3411,25 +3411,25 @@
     </row>
     <row r="58" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="B58" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="B58" s="2" t="s">
+      <c r="C58" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D58" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="C58" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D58" s="2" t="s">
+      <c r="E58" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="E58" s="2" t="s">
+      <c r="F58" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="F58" s="2" t="s">
-        <v>294</v>
-      </c>
       <c r="G58" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H58" s="2"/>
       <c r="I58" s="2"/>
@@ -3453,25 +3453,25 @@
     </row>
     <row r="59" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="B59" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="B59" s="2" t="s">
+      <c r="C59" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="C59" s="2" t="s">
+      <c r="D59" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="D59" s="2" t="s">
+      <c r="E59" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="E59" s="2" t="s">
+      <c r="F59" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="F59" s="2" t="s">
-        <v>300</v>
-      </c>
       <c r="G59" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H59" s="2"/>
       <c r="I59" s="2"/>
@@ -3495,25 +3495,25 @@
     </row>
     <row r="60" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="B60" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="B60" s="2" t="s">
+      <c r="C60" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="D60" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="C60" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="D60" s="2" t="s">
+      <c r="E60" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="E60" s="2" t="s">
+      <c r="F60" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="F60" s="2" t="s">
+      <c r="G60" s="3" t="s">
         <v>305</v>
-      </c>
-      <c r="G60" s="3" t="s">
-        <v>306</v>
       </c>
       <c r="H60" s="2"/>
       <c r="I60" s="2"/>
@@ -3537,25 +3537,25 @@
     </row>
     <row r="61" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="B61" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="B61" s="2" t="s">
+      <c r="C61" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F61" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="C61" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="D61" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E61" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F61" s="2" t="s">
-        <v>309</v>
-      </c>
       <c r="G61" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H61" s="2"/>
       <c r="I61" s="2"/>
@@ -3579,25 +3579,25 @@
     </row>
     <row r="62" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="B62" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="B62" s="2" t="s">
+      <c r="C62" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D62" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="C62" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D62" s="2" t="s">
+      <c r="E62" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="E62" s="2" t="s">
+      <c r="F62" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="F62" s="2" t="s">
-        <v>314</v>
-      </c>
       <c r="G62" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H62" s="2"/>
       <c r="I62" s="2"/>

</xml_diff>